<commit_message>
Updated a xlsx file
</commit_message>
<xml_diff>
--- a/gen_plates.xlsx
+++ b/gen_plates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angseung\VScode\kor_license_plate_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02790E84-33C9-4408-8050-E770FCD42014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C9A629-373D-4DFB-82FE-9FAFADC3EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6DB26215-BCC3-49EF-9635-7703A69967B3}"/>
   </bookViews>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1033FB53-8DB5-4AEC-A20F-0A8392146D43}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1236,12 +1236,12 @@
         <v>0</v>
       </c>
       <c r="D32" s="1">
-        <f>SUM($D$52:$D$85)*(35/34) / 10</f>
-        <v>5249.9999999999991</v>
+        <f>SUM($D$52:$D$85)*(35/34) / 15</f>
+        <v>3499.9999999999995</v>
       </c>
       <c r="E32" s="1">
         <f t="shared" si="1"/>
-        <v>5249.9999999999991</v>
+        <v>3499.9999999999995</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1255,12 +1255,12 @@
         <v>0</v>
       </c>
       <c r="D33" s="1">
-        <f>SUM($D$52:$D$85)*(35/34) / 10</f>
-        <v>5249.9999999999991</v>
+        <f>SUM($D$52:$D$85)*(35/34) / 15</f>
+        <v>3499.9999999999995</v>
       </c>
       <c r="E33" s="1">
         <f t="shared" si="1"/>
-        <v>5249.9999999999991</v>
+        <v>3499.9999999999995</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1328,12 +1328,12 @@
         <v>0</v>
       </c>
       <c r="D37" s="1">
-        <f>SUM($D$52:$D$85)*(35/34) / 10</f>
-        <v>5249.9999999999991</v>
+        <f>SUM($D$52:$D$85)*(35/34) / 15</f>
+        <v>3499.9999999999995</v>
       </c>
       <c r="E37" s="1">
         <f t="shared" si="1"/>
-        <v>5249.9999999999991</v>
+        <v>3499.9999999999995</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1401,12 +1401,12 @@
         <v>0</v>
       </c>
       <c r="D41" s="1">
-        <f>SUM($D$52:$D$85)*(35/34) / 10</f>
-        <v>5249.9999999999991</v>
+        <f>SUM($D$52:$D$85)*(35/34) / 15</f>
+        <v>3499.9999999999995</v>
       </c>
       <c r="E41" s="1">
         <f t="shared" si="1"/>
-        <v>5249.9999999999991</v>
+        <v>3499.9999999999995</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1474,12 +1474,12 @@
         <v>0</v>
       </c>
       <c r="D45" s="1">
-        <f>SUM($D$52:$D$85)*(35/34) / 10</f>
-        <v>5249.9999999999991</v>
+        <f>SUM($D$52:$D$85)*(35/34) / 15</f>
+        <v>3499.9999999999995</v>
       </c>
       <c r="E45" s="1">
         <f t="shared" si="1"/>
-        <v>5249.9999999999991</v>
+        <v>3499.9999999999995</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -2205,7 +2205,7 @@
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D86">
         <f>SUM(E12:E85)</f>
-        <v>124855</v>
+        <v>116105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>